<commit_message>
sn: burkina Faso updates.
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/septembre 2021/bf_lf_tas3_2_enrolement_202109.xlsx
+++ b/LF/TAS/Burkina Faso/septembre 2021/bf_lf_tas3_2_enrolement_202109.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Burkina Faso\septembre 2021\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CDC458-2E06-40F1-B8AD-C3EBB6C220D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -150,12 +156,6 @@
     <t>Entrer le code manuel</t>
   </si>
   <si>
-    <t>regex(.,'^[a-zA-Z]{2}[0-9]{4}$')</t>
-  </si>
-  <si>
-    <t>le format du code manuel manuel est de 2 lettres suivies de 4 chiffres</t>
-  </si>
-  <si>
     <t>${id_methode} = "Manuel"</t>
   </si>
   <si>
@@ -313,19 +313,19 @@
   </si>
   <si>
     <t>French</t>
+  </si>
+  <si>
+    <t>regex(.,'^[a-zA-Z]{2}[0-9]{5}$')</t>
+  </si>
+  <si>
+    <t>le format du code manuel manuel est de 2 lettres suivies de 5 chiffres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -362,152 +362,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,194 +382,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -723,264 +393,22 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1026,61 +454,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1338,31 +722,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6083333333333" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.7"/>
   <cols>
-    <col min="1" max="1" width="26.6083333333333" customWidth="1"/>
-    <col min="2" max="2" width="24.3833333333333" customWidth="1"/>
-    <col min="3" max="3" width="35.8833333333333" customWidth="1"/>
-    <col min="4" max="4" width="13.6083333333333" customWidth="1"/>
-    <col min="5" max="5" width="18.6083333333333" customWidth="1"/>
-    <col min="6" max="6" width="22.8833333333333" customWidth="1"/>
-    <col min="7" max="7" width="30.6083333333333" customWidth="1"/>
+    <col min="1" max="1" width="26.609375" customWidth="1"/>
+    <col min="2" max="2" width="24.38671875" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.609375" customWidth="1"/>
+    <col min="5" max="5" width="18.609375" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="30.609375" customWidth="1"/>
     <col min="9" max="9" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="37.5" spans="1:9">
+    <row r="1" spans="1:9" ht="36">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:9">
+    <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -1410,7 +794,7 @@
       </c>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="12" t="s">
         <v>19</v>
       </c>
@@ -1467,7 +851,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="30" spans="1:8">
+    <row r="6" spans="1:9" ht="31.35">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1489,7 +873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" ht="30" spans="1:8">
+    <row r="7" spans="1:9" ht="31.35">
       <c r="A7" s="12" t="s">
         <v>27</v>
       </c>
@@ -1511,7 +895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="12" t="s">
         <v>27</v>
       </c>
@@ -1572,7 +956,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" ht="45" spans="1:9">
+    <row r="11" spans="1:9" ht="47">
       <c r="A11" s="12" t="s">
         <v>27</v>
       </c>
@@ -1584,13 +968,13 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>12</v>
@@ -1602,18 +986,18 @@
         <v>27</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>12</v>
@@ -1625,17 +1009,17 @@
         <v>22</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="12" t="s">
@@ -1645,13 +1029,13 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1664,13 +1048,13 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1683,13 +1067,13 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1705,10 +1089,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
@@ -1717,20 +1101,20 @@
       <c r="H17" s="12"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:9">
       <c r="A18" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1743,30 +1127,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="$A6:$XFD19"/>
+      <selection activeCell="A6" sqref="A6:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6083333333333" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.7"/>
   <cols>
-    <col min="1" max="1" width="16.3833333333333" customWidth="1"/>
-    <col min="2" max="2" width="39.6083333333333" customWidth="1"/>
-    <col min="3" max="3" width="19.1083333333333" customWidth="1"/>
-    <col min="4" max="4" width="15.6083333333333" customWidth="1"/>
+    <col min="1" max="1" width="16.38671875" customWidth="1"/>
+    <col min="2" max="2" width="39.609375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.609375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -1775,241 +1157,241 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1">
+      <c r="A2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" s="2" customFormat="1" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="C2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1">
+      <c r="A3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1">
+      <c r="A4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" s="2" customFormat="1" spans="1:4">
-      <c r="A3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1">
+      <c r="A5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" s="2" customFormat="1" spans="1:4">
-      <c r="A4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1">
+      <c r="A6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" s="2" customFormat="1" spans="1:4">
-      <c r="A5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" s="3" customFormat="1" spans="1:4">
-      <c r="A6" s="5" t="s">
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1">
+      <c r="A7" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" s="3" customFormat="1" spans="1:4">
-      <c r="A7" s="5" t="s">
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1">
+      <c r="A8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1">
+      <c r="A9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1">
+      <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" s="3" customFormat="1" spans="1:4">
-      <c r="A8" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" s="3" customFormat="1">
+      <c r="A11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" s="3" customFormat="1">
+      <c r="A12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1">
+      <c r="A13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1">
+      <c r="A14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" s="3" customFormat="1" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" s="3" customFormat="1" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" s="3" customFormat="1" spans="1:4">
-      <c r="A11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" s="3" customFormat="1" spans="1:4">
-      <c r="A12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="C14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1">
+      <c r="A15" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" s="3" customFormat="1" spans="1:4">
-      <c r="A13" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" s="3" customFormat="1" spans="1:4">
-      <c r="A14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" s="3" customFormat="1" spans="1:4">
-      <c r="A15" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" s="3" customFormat="1" spans="1:4">
+    <row r="16" spans="1:4" s="3" customFormat="1">
       <c r="A16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" s="3" customFormat="1" spans="1:4">
+    <row r="17" spans="1:4" s="3" customFormat="1">
       <c r="A17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" s="3" customFormat="1" spans="1:4">
+    <row r="18" spans="1:4" s="3" customFormat="1">
       <c r="A18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" s="3" customFormat="1" spans="1:4">
+    <row r="19" spans="1:4" s="3" customFormat="1">
       <c r="A19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" s="3" customFormat="1" spans="1:4">
+    <row r="20" spans="1:4" s="3" customFormat="1">
       <c r="A20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" s="3" customFormat="1" spans="1:4">
+    <row r="21" spans="1:4" s="3" customFormat="1">
       <c r="A21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" s="3" customFormat="1" spans="1:4">
+    <row r="22" spans="1:4" s="3" customFormat="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:4">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:4">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:4">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:4">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:4">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:4">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:4">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:4">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:4">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:4">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1">
@@ -2050,53 +1432,51 @@
       <c r="C59" s="9"/>
     </row>
   </sheetData>
-  <sortState ref="A44:D58">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A44:D58">
     <sortCondition ref="B44:B58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6083333333333" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.7"/>
   <cols>
-    <col min="1" max="1" width="57.7166666666667" customWidth="1"/>
-    <col min="2" max="2" width="19.3833333333333" customWidth="1"/>
+    <col min="1" max="1" width="57.71875" customWidth="1"/>
+    <col min="2" max="2" width="19.38671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
         <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -2104,7 +1484,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>